<commit_message>
pilot analysis for DR~BS to get overlapping ROIs
</commit_message>
<xml_diff>
--- a/analy/pilot_analyis_ROIs.xlsx
+++ b/analy/pilot_analyis_ROIs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GenScotDepression/users/niamh/puberty_ABCD/ABCD_puberty_depression/analy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD271D2-85DF-D542-8170-52CE7E5E2E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D8BE83-257D-634E-8C2C-EC82E5BAD6F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6120" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{99C55ACA-72CF-884F-8C31-261502E5D86A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{99C55ACA-72CF-884F-8C31-261502E5D86A}"/>
   </bookViews>
   <sheets>
     <sheet name="Females_regional" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,10 @@
     <sheet name="SA" sheetId="4" r:id="rId4"/>
     <sheet name="FA" sheetId="5" r:id="rId5"/>
     <sheet name="MD" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Females_regional!$A$20:$G$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">vol!$B$3:$M$12</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="103">
   <si>
     <t>pt_f_INT</t>
   </si>
@@ -161,9 +163,6 @@
     <t>Superior Frontal Lobe</t>
   </si>
   <si>
-    <t>Superior Temporal Lobe</t>
-  </si>
-  <si>
     <t>Temporal Pole</t>
   </si>
   <si>
@@ -230,9 +229,6 @@
     <t>Model: Cortical volume ~ MDD/Depressive symptoms (Males and Females)</t>
   </si>
   <si>
-    <t xml:space="preserve">Middle Temporal Lobe </t>
-  </si>
-  <si>
     <t>Precentral gyrus</t>
   </si>
   <si>
@@ -282,6 +278,81 @@
   </si>
   <si>
     <t>Model: Cortical Volume ~ Pubertal Timing (Males)</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Limbic connections (cognition, episodic memory)</t>
+  </si>
+  <si>
+    <t>Cognitive, emotional function</t>
+  </si>
+  <si>
+    <t>Motor execution, reward, learning, emotion</t>
+  </si>
+  <si>
+    <t>Middle Temporal Gyrus</t>
+  </si>
+  <si>
+    <t>Inferior Parietal Gyrus</t>
+  </si>
+  <si>
+    <t>Caudal Middle Frontal Gyrus</t>
+  </si>
+  <si>
+    <t>Superior Frontal Gyrus</t>
+  </si>
+  <si>
+    <t>Superior Temporal Gyrus</t>
+  </si>
+  <si>
+    <t>vol.ASEG.aa~KSADS.MDD.p</t>
+  </si>
+  <si>
+    <t>dtimd_cst~KSADS.MDD.p</t>
+  </si>
+  <si>
+    <t>dtimd_pscs~KSADS.MDD.p</t>
+  </si>
+  <si>
+    <t>dtimd_scs~KSADS.MDD.p</t>
+  </si>
+  <si>
+    <t>thk.APARC.parstgris~KSADS.Depressive_symptoms_ever.y</t>
+  </si>
+  <si>
+    <t>dtimd_fscs~KSADS.MDD.p</t>
+  </si>
+  <si>
+    <t>dtimd_sifc~KSADS.MDD.p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corticospinal/pyramidal tract  </t>
+  </si>
+  <si>
+    <t>parstriangularis</t>
+  </si>
+  <si>
+    <t>striatal inferior frontal</t>
+  </si>
+  <si>
+    <t>Pubertal Timing ~ Regional Brain Structure (Cortical, subcortical, DTI)</t>
+  </si>
+  <si>
+    <t>Depression ~ Regional Brain Structure (Cortical, subcortical, DTI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> superior corticostriate-parietal cortex only</t>
+  </si>
+  <si>
+    <t>superior corticostriate-frontal tract only</t>
+  </si>
+  <si>
+    <t>Accumbens area</t>
+  </si>
+  <si>
+    <t>superior corticostriate tract</t>
   </si>
 </sst>
 </file>
@@ -291,10 +362,18 @@
   <numFmts count="1">
     <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -374,7 +453,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -396,6 +475,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,90 +625,94 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -972,10 +1061,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{37F91DAE-BB2D-3B47-AE40-52234FFE10CB}" name="Table3" displayName="Table3" ref="A1:G13" totalsRowShown="0" headerRowDxfId="9" dataDxfId="10">
-  <autoFilter ref="A1:G13" xr:uid="{37F91DAE-BB2D-3B47-AE40-52234FFE10CB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G13">
-    <sortCondition ref="G1:G13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{37F91DAE-BB2D-3B47-AE40-52234FFE10CB}" name="Table3" displayName="Table3" ref="A3:G15" totalsRowShown="0" headerRowDxfId="9" dataDxfId="10">
+  <autoFilter ref="A3:G15" xr:uid="{37F91DAE-BB2D-3B47-AE40-52234FFE10CB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:G15">
+    <sortCondition ref="G3:G15"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{4F59B139-DEA7-D34C-A1F4-CBFB8CDC49CD}" name="Model Name" dataDxfId="17"/>
@@ -1306,10 +1395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE781A1B-C088-084F-98E9-24A90144598A}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1319,306 +1408,535 @@
     <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="3">
-        <v>-0.21579506694499201</v>
-      </c>
-      <c r="D2" s="3">
-        <v>5.5512911885356002E-2</v>
-      </c>
-      <c r="E2" s="3">
-        <v>-3.8872950385064899</v>
-      </c>
-      <c r="F2" s="3">
-        <v>1.23041875267057E-4</v>
-      </c>
-      <c r="G2" s="3">
-        <v>2.4608379999999999E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="3">
-        <v>-0.149810562169721</v>
-      </c>
-      <c r="D3" s="3">
-        <v>3.97227835111299E-2</v>
-      </c>
-      <c r="E3" s="3">
-        <v>-3.7714014207424702</v>
-      </c>
-      <c r="F3" s="3">
-        <v>1.9105184841521899E-4</v>
-      </c>
-      <c r="G3" s="3">
-        <v>6.4957629999999999E-3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="C4" s="3">
-        <v>-0.130590316971677</v>
+        <v>-0.21579506694499201</v>
       </c>
       <c r="D4" s="3">
-        <v>3.7541616069141602E-2</v>
+        <v>5.5512911885356002E-2</v>
       </c>
       <c r="E4" s="3">
-        <v>-3.47854809263311</v>
+        <v>-3.8872950385064899</v>
       </c>
       <c r="F4" s="3">
-        <v>5.6888784190949201E-4</v>
+        <v>1.23041875267057E-4</v>
       </c>
       <c r="G4" s="3">
-        <v>1.7911775000000001E-2</v>
+        <v>2.4608379999999999E-3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C5" s="3">
-        <v>-0.12580485790913201</v>
+        <v>-0.149810562169721</v>
       </c>
       <c r="D5" s="3">
-        <v>3.8077172491759001E-2</v>
+        <v>3.97227835111299E-2</v>
       </c>
       <c r="E5" s="3">
-        <v>-3.3039443235014399</v>
+        <v>-3.7714014207424702</v>
       </c>
       <c r="F5" s="3">
-        <v>1.0536338346403299E-3</v>
+        <v>1.9105184841521899E-4</v>
       </c>
       <c r="G5" s="3">
-        <v>1.7911775000000001E-2</v>
+        <v>6.4957629999999999E-3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="C6" s="3">
-        <v>-0.17502811374494001</v>
+        <v>-0.130590316971677</v>
       </c>
       <c r="D6" s="3">
-        <v>5.6015506927799302E-2</v>
+        <v>3.7541616069141602E-2</v>
       </c>
       <c r="E6" s="3">
-        <v>-3.1246367897828802</v>
+        <v>-3.47854809263311</v>
       </c>
       <c r="F6" s="3">
-        <v>1.9416850184106899E-3</v>
+        <v>5.6888784190949201E-4</v>
       </c>
       <c r="G6" s="3">
-        <v>1.9416849999999999E-2</v>
+        <v>1.7911775000000001E-2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C7" s="3">
-        <v>-0.13275058975131501</v>
+        <v>-0.12580485790913201</v>
       </c>
       <c r="D7" s="3">
-        <v>4.4845912090474498E-2</v>
+        <v>3.8077172491759001E-2</v>
       </c>
       <c r="E7" s="3">
-        <v>-2.9601491766629202</v>
+        <v>-3.3039443235014399</v>
       </c>
       <c r="F7" s="3">
-        <v>3.3009538346892098E-3</v>
+        <v>1.0536338346403299E-3</v>
       </c>
       <c r="G7" s="3">
-        <v>2.6407631000000001E-2</v>
+        <v>1.7911775000000001E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C8" s="3">
-        <v>-0.13102856819884501</v>
+        <v>-0.17502811374494001</v>
       </c>
       <c r="D8" s="3">
-        <v>4.6062294039718399E-2</v>
+        <v>5.6015506927799302E-2</v>
       </c>
       <c r="E8" s="3">
-        <v>-2.8445949323727202</v>
+        <v>-3.1246367897828802</v>
       </c>
       <c r="F8" s="3">
-        <v>4.7305054442454897E-3</v>
+        <v>1.9416850184106899E-3</v>
       </c>
       <c r="G8" s="3">
-        <v>3.1536702999999999E-2</v>
+        <v>1.9416849999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C9" s="3">
-        <v>-0.13109117443104201</v>
+        <v>-0.13275058975131501</v>
       </c>
       <c r="D9" s="3">
-        <v>4.5318476541957503E-2</v>
+        <v>4.4845912090474498E-2</v>
       </c>
       <c r="E9" s="3">
-        <v>-2.8926650768957902</v>
+        <v>-2.9601491766629202</v>
       </c>
       <c r="F9" s="3">
-        <v>4.0631358396419201E-3</v>
+        <v>3.3009538346892098E-3</v>
       </c>
       <c r="G9" s="3">
-        <v>3.2505087000000002E-2</v>
+        <v>2.6407631000000001E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C10" s="3">
-        <v>-0.11381890725735699</v>
+        <v>-0.13102856819884501</v>
       </c>
       <c r="D10" s="3">
-        <v>3.9817827531138002E-2</v>
+        <v>4.6062294039718399E-2</v>
       </c>
       <c r="E10" s="3">
-        <v>-2.8584911411439902</v>
+        <v>-2.8445949323727202</v>
       </c>
       <c r="F10" s="3">
-        <v>4.5160029897856196E-3</v>
+        <v>4.7305054442454897E-3</v>
       </c>
       <c r="G10" s="3">
-        <v>5.1181366999999998E-2</v>
+        <v>3.1536702999999999E-2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C11" s="3">
-        <v>0.15619623770648899</v>
+        <v>-0.13109117443104201</v>
       </c>
       <c r="D11" s="3">
-        <v>5.2319462846438701E-2</v>
+        <v>4.5318476541957503E-2</v>
       </c>
       <c r="E11" s="3">
-        <v>2.9854327473685198</v>
+        <v>-2.8926650768957902</v>
       </c>
       <c r="F11" s="3">
-        <v>3.04803888929601E-3</v>
+        <v>4.0631358396419201E-3</v>
       </c>
       <c r="G11" s="3">
-        <v>6.0960778E-2</v>
+        <v>3.2505087000000002E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="C12" s="3">
-        <v>-0.11170892961390499</v>
+        <v>-0.11381890725735699</v>
       </c>
       <c r="D12" s="3">
-        <v>3.9036875772894497E-2</v>
+        <v>3.9817827531138002E-2</v>
       </c>
       <c r="E12" s="3">
-        <v>-2.86162576799935</v>
+        <v>-2.8584911411439902</v>
       </c>
       <c r="F12" s="3">
-        <v>4.4726271443097003E-3</v>
+        <v>4.5160029897856196E-3</v>
       </c>
       <c r="G12" s="3">
-        <v>7.0915986E-2</v>
+        <v>5.1181366999999998E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.15619623770648899</v>
+      </c>
+      <c r="D13" s="3">
+        <v>5.2319462846438701E-2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>2.9854327473685198</v>
+      </c>
+      <c r="F13" s="3">
+        <v>3.04803888929601E-3</v>
+      </c>
+      <c r="G13" s="3">
+        <v>6.0960778E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="3">
+        <v>-0.11170892961390499</v>
+      </c>
+      <c r="D14" s="3">
+        <v>3.9036875772894497E-2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>-2.86162576799935</v>
+      </c>
+      <c r="F14" s="3">
+        <v>4.4726271443097003E-3</v>
+      </c>
+      <c r="G14" s="3">
+        <v>7.0915986E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="3">
+      <c r="B15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="3">
         <v>0.12674479856736101</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D15" s="3">
         <v>4.2612972807056899E-2</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E15" s="3">
         <v>2.9743242542883901</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F15" s="3">
         <v>3.1533812925872602E-3</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G15" s="3">
         <v>0.114392223</v>
       </c>
     </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="47"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+    </row>
+    <row r="20" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="48" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="2">
+        <v>-0.147006626034761</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3.9803529639112503E-2</v>
+      </c>
+      <c r="E21" s="2">
+        <v>-3.69330628131799</v>
+      </c>
+      <c r="F21" s="2">
+        <v>2.5163657626043598E-4</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1.9376020000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.129282162632082</v>
+      </c>
+      <c r="D22" s="2">
+        <v>3.9433680415157803E-2</v>
+      </c>
+      <c r="E22" s="2">
+        <v>3.2784706187958998</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1.13739742064979E-3</v>
+      </c>
+      <c r="G22" s="2">
+        <v>5.4769239999999997E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.15335970709806501</v>
+      </c>
+      <c r="D23" s="2">
+        <v>4.8187297480228403E-2</v>
+      </c>
+      <c r="E23" s="2">
+        <v>3.1825753905578398</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1.5767430957132199E-3</v>
+      </c>
+      <c r="G23" s="2">
+        <v>5.4769239999999997E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.14455600114690001</v>
+      </c>
+      <c r="D24" s="2">
+        <v>4.6963415640034797E-2</v>
+      </c>
+      <c r="E24" s="2">
+        <v>3.07805552847547</v>
+      </c>
+      <c r="F24" s="2">
+        <v>2.2308239186179702E-3</v>
+      </c>
+      <c r="G24" s="2">
+        <v>5.4769239999999997E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.115552791501083</v>
+      </c>
+      <c r="D25" s="2">
+        <v>3.7731372496049603E-2</v>
+      </c>
+      <c r="E25" s="2">
+        <v>3.0625122771025799</v>
+      </c>
+      <c r="F25" s="2">
+        <v>2.3409801790124501E-3</v>
+      </c>
+      <c r="G25" s="2">
+        <v>7.9593330000000004E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.13613824305904201</v>
+      </c>
+      <c r="D26" s="2">
+        <v>4.6294936850826397E-2</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2.9406724000448099</v>
+      </c>
+      <c r="F26" s="2">
+        <v>3.4701783730932399E-3</v>
+      </c>
+      <c r="G26" s="2">
+        <v>5.4769239999999997E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.114959540649913</v>
+      </c>
+      <c r="D27" s="2">
+        <v>3.9366344167140202E-2</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2.9202493419714499</v>
+      </c>
+      <c r="F27" s="2">
+        <v>3.70062400606091E-3</v>
+      </c>
+      <c r="G27" s="2">
+        <v>5.4769239999999997E-2</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A20:G20" xr:uid="{DE781A1B-C088-084F-98E9-24A90144598A}"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="A18:G19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1631,7 +1949,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:G5"/>
+      <selection activeCell="A2" sqref="A1:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1646,7 +1964,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>15</v>
@@ -1669,7 +1987,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C2" s="2">
         <v>-0.130308434925691</v>
@@ -1715,7 +2033,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4" s="2">
         <v>-0.114133955940351</v>
@@ -1738,7 +2056,7 @@
         <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C5" s="2">
         <v>-0.109850303870523</v>
@@ -1768,8 +2086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70CCD8DC-E71A-5241-8308-A0FD1A7E099E}">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1786,7 +2104,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -1801,7 +2119,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>25</v>
@@ -1848,7 +2166,7 @@
     </row>
     <row r="5" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="C5" s="10">
         <v>-2.5901226865233901E-2</v>
@@ -1924,7 +2242,7 @@
     </row>
     <row r="7" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="10" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="C7" s="10">
         <v>-2.0686532463047351E-2</v>
@@ -1963,7 +2281,7 @@
     <row r="8" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="46"/>
       <c r="B8" s="46" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="C8" s="46">
         <v>-1.5677152913838015E-2</v>
@@ -2039,7 +2357,7 @@
     </row>
     <row r="10" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="10" t="s">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="C10" s="10">
         <v>-2.1519624867399334E-2</v>
@@ -2077,7 +2395,7 @@
     </row>
     <row r="11" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="10" t="s">
-        <v>39</v>
+        <v>86</v>
       </c>
       <c r="C11" s="10">
         <v>-2.1060700997669834E-2</v>
@@ -2115,7 +2433,7 @@
     </row>
     <row r="12" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="10">
         <v>-3.2890912775612957E-2</v>
@@ -2153,7 +2471,7 @@
     </row>
     <row r="17" spans="1:18" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
@@ -2168,7 +2486,7 @@
     </row>
     <row r="18" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="37" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>25</v>
@@ -2229,7 +2547,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="43" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="C21" s="44">
         <v>-0.12580485790913201</v>
@@ -2249,7 +2567,7 @@
         <v>0</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C22" s="17">
         <v>-0.11381890725735699</v>
@@ -2269,7 +2587,7 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B24" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
@@ -2287,7 +2605,7 @@
         <v>0</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C25" s="17">
         <v>-0.13109117443104201</v>
@@ -2304,7 +2622,7 @@
     </row>
     <row r="30" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="B30" s="24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C30" s="24"/>
       <c r="D30" s="24"/>
@@ -2319,7 +2637,7 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="37" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>25</v>
@@ -2397,7 +2715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{474815C6-3891-5B49-88A6-61B76674803E}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -2410,7 +2728,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
@@ -2598,7 +2916,7 @@
     <row r="11" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="22"/>
       <c r="B11" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
@@ -2629,7 +2947,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="23" t="s">
@@ -2656,7 +2974,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C14" s="17">
         <v>-0.149810562169721</v>
@@ -2708,7 +3026,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C16" s="27">
         <v>0.12674479856736101</v>
@@ -2746,7 +3064,7 @@
     <row r="18" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="22"/>
       <c r="B18" s="24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C18" s="24"/>
       <c r="D18" s="24"/>
@@ -2761,7 +3079,7 @@
     </row>
     <row r="19" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="37" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>25</v>
@@ -2868,7 +3186,7 @@
   <sheetData>
     <row r="1" spans="1:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
@@ -2892,7 +3210,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>25</v>
@@ -2940,7 +3258,7 @@
     </row>
     <row r="5" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="11">
         <v>-2.7564766192200208E-2</v>
@@ -2978,7 +3296,7 @@
     </row>
     <row r="6" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="11">
         <v>-4.0065938874918813E-2</v>
@@ -3016,7 +3334,7 @@
     </row>
     <row r="7" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" s="11">
         <v>-3.331568136295094E-2</v>
@@ -3054,7 +3372,7 @@
     </row>
     <row r="8" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="11">
         <v>-4.1612339811237756E-2</v>
@@ -3092,7 +3410,7 @@
     </row>
     <row r="9" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="11">
         <v>-2.2060051008089377E-2</v>
@@ -3130,7 +3448,7 @@
     </row>
     <row r="10" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" s="11">
         <v>-2.6522408515554749E-2</v>
@@ -3173,7 +3491,7 @@
     <row r="15" spans="1:21" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22"/>
       <c r="B15" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C15" s="24"/>
       <c r="D15" s="24"/>
@@ -3188,7 +3506,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>25</v>
@@ -3231,7 +3549,7 @@
         <v>0</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C18" s="17">
         <v>0.15619623770648899</v>
@@ -3278,7 +3596,7 @@
   <sheetData>
     <row r="1" spans="2:21" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -3346,7 +3664,7 @@
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5">
         <v>1.1317251309502943E-3</v>
@@ -3384,7 +3702,7 @@
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6">
         <v>7.2878269742865966E-3</v>
@@ -3422,7 +3740,7 @@
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7">
         <v>-4.1358002283423531E-3</v>
@@ -3460,7 +3778,7 @@
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8">
         <v>1.3751974061924968E-3</v>
@@ -3498,7 +3816,7 @@
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9">
         <v>-8.048463519954821E-3</v>
@@ -3536,7 +3854,7 @@
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10">
         <v>-1.4141222298100034E-3</v>
@@ -3574,7 +3892,7 @@
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11">
         <v>4.6317163558312899E-3</v>
@@ -3612,7 +3930,7 @@
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12">
         <v>-7.5202471108171357E-3</v>
@@ -3650,7 +3968,7 @@
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13">
         <v>1.3919635472334388E-2</v>
@@ -3688,7 +4006,7 @@
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14">
         <v>9.005698793529927E-3</v>
@@ -3726,7 +4044,7 @@
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15">
         <v>1.6893596106884564E-2</v>
@@ -3764,7 +4082,7 @@
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16">
         <v>8.9686870174137973E-3</v>
@@ -3802,7 +4120,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17">
         <v>1.8903755256777469E-3</v>
@@ -3840,7 +4158,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18">
         <v>1.5149999421964733E-2</v>
@@ -3879,7 +4197,7 @@
     <row r="21" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="22"/>
       <c r="B21" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C21" s="24"/>
       <c r="D21" s="24"/>
@@ -3894,7 +4212,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B22" s="25" t="s">
         <v>25</v>
@@ -3937,7 +4255,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" s="17">
         <v>-0.21579506694499201</v>
@@ -3957,7 +4275,7 @@
         <v>0</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C25" s="17">
         <v>-0.17502811374494001</v>
@@ -3977,7 +4295,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C26" s="17">
         <v>-0.13102856819884501</v>
@@ -4005,4 +4323,109 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF950475-37A5-FE47-ACE0-5BDE11B9A7D1}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="44.33203125" customWidth="1"/>
+    <col min="2" max="2" width="45.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
pilot analysis updates with CI
</commit_message>
<xml_diff>
--- a/analy/pilot_analyis_ROIs.xlsx
+++ b/analy/pilot_analyis_ROIs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GenScotDepression/users/niamh/puberty_ABCD/ABCD_puberty_depression/analy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D8BE83-257D-634E-8C2C-EC82E5BAD6F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648E3064-D1D9-1D45-B744-668BAB8DF0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{99C55ACA-72CF-884F-8C31-261502E5D86A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{99C55ACA-72CF-884F-8C31-261502E5D86A}"/>
   </bookViews>
   <sheets>
     <sheet name="Females_regional" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Females_regional!$A$20:$G$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Males_regional!$A$13:$G$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">vol!$B$3:$M$12</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="112">
   <si>
     <t>pt_f_INT</t>
   </si>
@@ -343,9 +344,6 @@
     <t>Depression ~ Regional Brain Structure (Cortical, subcortical, DTI)</t>
   </si>
   <si>
-    <t xml:space="preserve"> superior corticostriate-parietal cortex only</t>
-  </si>
-  <si>
     <t>superior corticostriate-frontal tract only</t>
   </si>
   <si>
@@ -353,6 +351,36 @@
   </si>
   <si>
     <t>superior corticostriate tract</t>
+  </si>
+  <si>
+    <t>superior corticostriate-parietal cortex only</t>
+  </si>
+  <si>
+    <t>thk.APARC.parahpal~KSADS.Depressive_symptoms_ever.p</t>
+  </si>
+  <si>
+    <t>dtifa_tslf~KSADS.MDD.y</t>
+  </si>
+  <si>
+    <t>dtifa_slf~KSADS.MDD.y</t>
+  </si>
+  <si>
+    <t>sulc.APARC.paracn~KSADS.Depressive_symptoms_ever.y</t>
+  </si>
+  <si>
+    <t>dtifa_pslf~KSADS.Depressive_symptoms_ever.y</t>
+  </si>
+  <si>
+    <t>temporal superior longitudinal fasiculus</t>
+  </si>
+  <si>
+    <t>superior longitudinal fasiculus</t>
+  </si>
+  <si>
+    <t>parietal superior longitudinal fasiculus</t>
+  </si>
+  <si>
+    <t>Parahippocampal</t>
   </si>
 </sst>
 </file>
@@ -453,7 +481,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,6 +510,12 @@
       <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
       </patternFill>
     </fill>
     <fill>
@@ -625,7 +659,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -646,27 +680,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -675,7 +709,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -694,14 +728,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -712,7 +746,10 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1080,10 +1117,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{94559056-C672-F641-9AC1-B6C43E2F299C}" name="Table4" displayName="Table4" ref="A1:G5" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:G5" xr:uid="{94559056-C672-F641-9AC1-B6C43E2F299C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G5">
-    <sortCondition ref="F1:F5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{94559056-C672-F641-9AC1-B6C43E2F299C}" name="Table4" displayName="Table4" ref="A3:G7" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A3:G7" xr:uid="{94559056-C672-F641-9AC1-B6C43E2F299C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:G7">
+    <sortCondition ref="F3:F7"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{E8D9F4DC-C3AF-B144-9A8E-39D1D4441B91}" name="Model Name" dataDxfId="8"/>
@@ -1397,8 +1434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE781A1B-C088-084F-98E9-24A90144598A}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1775,7 +1812,7 @@
         <v>87</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C21" s="2">
         <v>-0.147006626034761</v>
@@ -1821,7 +1858,7 @@
         <v>89</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C23" s="2">
         <v>0.15335970709806501</v>
@@ -1844,7 +1881,7 @@
         <v>90</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C24" s="2">
         <v>0.14455600114690001</v>
@@ -1890,7 +1927,7 @@
         <v>92</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C26" s="2">
         <v>0.13613824305904201</v>
@@ -1946,135 +1983,319 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629E7D07-E512-474F-BE9D-F1D1A7F46226}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="31" customWidth="1"/>
+    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="2" max="2" width="38" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="2">
-        <v>-0.130308434925691</v>
-      </c>
-      <c r="D2" s="2">
-        <v>4.4624439925911703E-2</v>
-      </c>
-      <c r="E2" s="2">
-        <v>-2.9201136225359199</v>
-      </c>
-      <c r="F2" s="2">
-        <v>3.6916788935156598E-3</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0.12551708</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.11961066440562799</v>
-      </c>
-      <c r="D3" s="2">
-        <v>4.1100821753211302E-2</v>
-      </c>
-      <c r="E3" s="2">
-        <v>2.9101769576245098</v>
-      </c>
-      <c r="F3" s="2">
-        <v>3.8231843784941799E-3</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0.13122176999999999</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="2">
-        <v>-0.114133955940351</v>
+        <v>-0.130308434925691</v>
       </c>
       <c r="D4" s="2">
-        <v>4.0188049839942799E-2</v>
+        <v>4.4624439925911703E-2</v>
       </c>
       <c r="E4" s="2">
-        <v>-2.8399973722266498</v>
+        <v>-2.9201136225359199</v>
       </c>
       <c r="F4" s="2">
-        <v>4.7514846393276796E-3</v>
+        <v>3.6916788935156598E-3</v>
       </c>
       <c r="G4" s="2">
-        <v>0.16155048</v>
+        <v>0.12551708</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.11961066440562799</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4.1100821753211302E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2.9101769576245098</v>
+      </c>
+      <c r="F5" s="2">
+        <v>3.8231843784941799E-3</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.13122176999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="2">
+        <v>-0.114133955940351</v>
+      </c>
+      <c r="D6" s="2">
+        <v>4.0188049839942799E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>-2.8399973722266498</v>
+      </c>
+      <c r="F6" s="2">
+        <v>4.7514846393276796E-3</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.16155048</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C7" s="2">
         <v>-0.109850303870523</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D7" s="2">
         <v>3.8825168500808402E-2</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E7" s="2">
         <v>-2.8293580713818698</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F7" s="2">
         <v>4.9089656559994001E-3</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G7" s="2">
         <v>0.20617656000000001</v>
       </c>
     </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="47"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="51" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="2">
+        <v>-0.159654192419423</v>
+      </c>
+      <c r="D14" s="2">
+        <v>4.3257149576602802E-2</v>
+      </c>
+      <c r="E14" s="2">
+        <v>-3.6908162923841301</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2.5178228534920199E-4</v>
+      </c>
+      <c r="G14" s="2">
+        <v>2.2156840000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="2">
+        <v>-0.13147713988864901</v>
+      </c>
+      <c r="D15" s="2">
+        <v>3.84576648052255E-2</v>
+      </c>
+      <c r="E15" s="2">
+        <v>-3.41874995672603</v>
+      </c>
+      <c r="F15" s="2">
+        <v>6.9040522592329597E-4</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1.38081E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="2">
+        <v>-0.12089192935819899</v>
+      </c>
+      <c r="D16" s="2">
+        <v>3.8672222834951697E-2</v>
+      </c>
+      <c r="E16" s="2">
+        <v>-3.1260662174540901</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1.89438931025947E-3</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1.8943890000000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.112518642498611</v>
+      </c>
+      <c r="D17" s="2">
+        <v>3.76911707257045E-2</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2.9852785236483999</v>
+      </c>
+      <c r="F17" s="2">
+        <v>2.9922929008776699E-3</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.10173796</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" s="2">
+        <v>-0.114740791343866</v>
+      </c>
+      <c r="D18" s="2">
+        <v>3.9599447235484801E-2</v>
+      </c>
+      <c r="E18" s="2">
+        <v>-2.89753517672963</v>
+      </c>
+      <c r="F18" s="2">
+        <v>3.9574395126503901E-3</v>
+      </c>
+      <c r="G18" s="2">
+        <v>7.9148789999999997E-2</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A13:G13" xr:uid="{629E7D07-E512-474F-BE9D-F1D1A7F46226}"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="A11:G12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>